<commit_message>
finishing semua laporan keuangan
Co-authored-by: Anto Wiranto <antowrnto11@gmail.com>
Co-authored-by: Sri Heryanti <Sriheryanti@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/storage/laporan-kinerja2022.xlsx
+++ b/storage/laporan-kinerja2022.xlsx
@@ -512,13 +512,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>